<commit_message>
add ModelRockets.us tube size info
</commit_message>
<xml_diff>
--- a/data/body_tube_data.xlsx
+++ b/data/body_tube_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24080" windowHeight="29480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24080" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="279">
   <si>
     <t>ID inches</t>
   </si>
@@ -748,9 +748,6 @@
     <t>C38-400</t>
   </si>
   <si>
-    <t>dimensions based on .003 clearance and .061 wall</t>
-  </si>
-  <si>
     <t>C22-400</t>
   </si>
   <si>
@@ -763,10 +760,160 @@
     <t>C39-800HD</t>
   </si>
   <si>
-    <t>dimensions based on .003 clearance and .115 wall</t>
-  </si>
-  <si>
     <t>FC26</t>
+  </si>
+  <si>
+    <t>DISCOUNT ROCKETRY (modelrockets.us)</t>
+  </si>
+  <si>
+    <t>TC-38mm</t>
+  </si>
+  <si>
+    <t>TC-29mm</t>
+  </si>
+  <si>
+    <t>TC-24mm</t>
+  </si>
+  <si>
+    <t>TC-1.90</t>
+  </si>
+  <si>
+    <t>MR-11011 3.0" len</t>
+  </si>
+  <si>
+    <t>MR-11013 6.0" len</t>
+  </si>
+  <si>
+    <t>TC-3.90</t>
+  </si>
+  <si>
+    <t>TC-54mm</t>
+  </si>
+  <si>
+    <t>T-38mm</t>
+  </si>
+  <si>
+    <t>dimensions based on .010 clearance and .061 wall</t>
+  </si>
+  <si>
+    <t>dimensions based on .010 clearance and .115 wall</t>
+  </si>
+  <si>
+    <t>T-29mm</t>
+  </si>
+  <si>
+    <t>T-24mm</t>
+  </si>
+  <si>
+    <t>T-1.90</t>
+  </si>
+  <si>
+    <t>T-54mm</t>
+  </si>
+  <si>
+    <t>T-2.56</t>
+  </si>
+  <si>
+    <t>T-3.00</t>
+  </si>
+  <si>
+    <t>T-3.90</t>
+  </si>
+  <si>
+    <t>MR-06032 34", MR-06031 12"</t>
+  </si>
+  <si>
+    <t>MR-06018 13", MR-06019 34", MR-06016 7.0", MR-06017 7.5"</t>
+  </si>
+  <si>
+    <t>MR-06020 6.75", MR-06021 13.3", MR-06022 34"</t>
+  </si>
+  <si>
+    <t>MR-06033 34"</t>
+  </si>
+  <si>
+    <t>MR-06034 16", MR-06035 34"</t>
+  </si>
+  <si>
+    <t>MR-06026 34", MR-06025 15", MR-06024 11", MR-06023 7.5"</t>
+  </si>
+  <si>
+    <t>T-5.38</t>
+  </si>
+  <si>
+    <t>MR-06036 26", MR-06037 34", MR-06038 54"</t>
+  </si>
+  <si>
+    <t>MR-06027 8.5", MR-06028 12.75", MR-06029 25.75", MR-06030 34"</t>
+  </si>
+  <si>
+    <t>Oddly there is no 1.9" tube, though there is a coupler MR-11011</t>
+  </si>
+  <si>
+    <t>Cardboard Airframe - LOC exact compatible</t>
+  </si>
+  <si>
+    <t>Cardboard Couplers - not exact LOC sizes</t>
+  </si>
+  <si>
+    <t>ERROR: sizes don't line up against tube 2.56 ID</t>
+  </si>
+  <si>
+    <t>MR-11012 3.75" len, 0.005 clearance</t>
+  </si>
+  <si>
+    <t>MR-11010 4.0" len, 0.010 clearance</t>
+  </si>
+  <si>
+    <t>MR-11009 for 2.0" len, 0.005 clearance</t>
+  </si>
+  <si>
+    <t>MR-11008 for 2.0" len, 0.005 clearance</t>
+  </si>
+  <si>
+    <t>MR-11014 6.0" len, 0.005 clearance</t>
+  </si>
+  <si>
+    <t>MR-11015 6.0" len, 0.005 clearaance</t>
+  </si>
+  <si>
+    <t>no matching tube! Zero clearance vs Aerotech tube ID</t>
+  </si>
+  <si>
+    <t>Charlie Savoie confirmed at NSL 2017 that AT has never had a 3.0" tube</t>
+  </si>
+  <si>
+    <t>minor: zero clearance vs BT-1.52 tube ID</t>
+  </si>
+  <si>
+    <t>only 0.002 clearance</t>
+  </si>
+  <si>
+    <t>.005 clearance</t>
+  </si>
+  <si>
+    <t>.010 clearance</t>
+  </si>
+  <si>
+    <t>.016 clearance</t>
+  </si>
+  <si>
+    <t>.008 clearance</t>
+  </si>
+  <si>
+    <t>.007 clearance</t>
+  </si>
+  <si>
+    <t>.002 clearance</t>
+  </si>
+  <si>
+    <t>.000 clearance</t>
+  </si>
+  <si>
+    <t>.013 clearance</t>
+  </si>
+  <si>
+    <t>large clearance 0.013, is this right?</t>
   </si>
 </sst>
 </file>
@@ -863,9 +1010,67 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="196">
+  <cellStyleXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1080,7 +1285,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="196">
+  <cellStyles count="254">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1178,6 +1383,35 @@
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1276,6 +1510,35 @@
     <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1605,10 +1868,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M212"/>
+  <dimension ref="A1:M239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <pane ySplit="5060" topLeftCell="A216"/>
+      <selection activeCell="A130" sqref="A130"/>
+      <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3456,12 +3721,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" ht="30">
       <c r="A89" s="1" t="s">
         <v>98</v>
       </c>
       <c r="H89" t="s">
         <v>106</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3876,7 +4144,7 @@
         <v>1.5170000000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -3902,7 +4170,7 @@
         <v>2.137</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -3928,7 +4196,7 @@
         <v>2.5569999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -3954,7 +4222,7 @@
         <v>2.9969999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -3980,7 +4248,7 @@
         <v>3.8969999999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -4006,7 +4274,7 @@
         <v>5.3769999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -4032,7 +4300,7 @@
         <v>7.5119999999999996</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -4058,7 +4326,7 @@
         <v>2.9969999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4084,7 +4352,7 @@
         <v>3.8969999999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>128</v>
       </c>
@@ -4109,8 +4377,14 @@
         <f t="shared" ref="G123:G130" si="32">B123-E123</f>
         <v>1.0030000000000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="H123" t="s">
+        <v>277</v>
+      </c>
+      <c r="I123" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>129</v>
       </c>
@@ -4135,8 +4409,14 @@
         <f t="shared" si="32"/>
         <v>1.395</v>
       </c>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="H124" t="s">
+        <v>276</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>130</v>
       </c>
@@ -4161,8 +4441,14 @@
         <f t="shared" si="32"/>
         <v>2.0139999999999998</v>
       </c>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="H125" t="s">
+        <v>275</v>
+      </c>
+      <c r="I125" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>131</v>
       </c>
@@ -4187,8 +4473,11 @@
         <f t="shared" si="32"/>
         <v>2.476</v>
       </c>
-    </row>
-    <row r="127" spans="1:7">
+      <c r="H126" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>132</v>
       </c>
@@ -4213,8 +4502,11 @@
         <f t="shared" si="32"/>
         <v>2.8769999999999998</v>
       </c>
-    </row>
-    <row r="128" spans="1:7">
+      <c r="H127" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>133</v>
       </c>
@@ -4239,6 +4531,9 @@
         <f t="shared" si="32"/>
         <v>3.8083999999999998</v>
       </c>
+      <c r="H128" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
@@ -4265,6 +4560,9 @@
         <f t="shared" si="32"/>
         <v>5.2690000000000001</v>
       </c>
+      <c r="H129" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
@@ -4291,6 +4589,9 @@
         <f t="shared" si="32"/>
         <v>7.3949999999999996</v>
       </c>
+      <c r="H130" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
@@ -5345,7 +5646,7 @@
     </row>
     <row r="186" spans="1:9">
       <c r="A186" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B186" s="5">
         <v>2.375</v>
@@ -5792,28 +6093,28 @@
         <v>222</v>
       </c>
       <c r="B208" s="5">
-        <v>1.4</v>
+        <v>1.393</v>
       </c>
       <c r="C208" s="5">
-        <v>1.522</v>
+        <v>1.5149999999999999</v>
       </c>
       <c r="D208" s="5">
         <f t="shared" ref="D208" si="111">(C208-B208)/2</f>
-        <v>6.1000000000000054E-2</v>
+        <v>6.0999999999999943E-2</v>
       </c>
       <c r="E208" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F208" s="5">
         <f t="shared" ref="F208" si="112">C208+E208</f>
-        <v>1.5249999999999999</v>
+        <v>1.5179999999999998</v>
       </c>
       <c r="G208" s="5">
         <f t="shared" ref="G208" si="113">B208-E208</f>
-        <v>1.397</v>
+        <v>1.3900000000000001</v>
       </c>
       <c r="H208" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="I208" s="6" t="s">
         <v>179</v>
@@ -5821,31 +6122,31 @@
     </row>
     <row r="209" spans="1:9">
       <c r="A209" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B209" s="5">
-        <v>2.0499999999999998</v>
+        <v>2.0430000000000001</v>
       </c>
       <c r="C209" s="5">
-        <v>2.1720000000000002</v>
+        <v>2.165</v>
       </c>
       <c r="D209" s="5">
         <f t="shared" ref="D209" si="114">(C209-B209)/2</f>
-        <v>6.1000000000000165E-2</v>
+        <v>6.0999999999999943E-2</v>
       </c>
       <c r="E209" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F209" s="5">
         <f t="shared" ref="F209" si="115">C209+E209</f>
-        <v>2.1750000000000003</v>
+        <v>2.1680000000000001</v>
       </c>
       <c r="G209" s="5">
         <f t="shared" ref="G209" si="116">B209-E209</f>
-        <v>2.0469999999999997</v>
+        <v>2.04</v>
       </c>
       <c r="H209" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="I209" s="6" t="s">
         <v>179</v>
@@ -5853,31 +6154,31 @@
     </row>
     <row r="210" spans="1:9">
       <c r="A210" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B210" s="5">
-        <v>2.4329999999999998</v>
+        <v>2.4260000000000002</v>
       </c>
       <c r="C210" s="5">
-        <v>2.5550000000000002</v>
+        <v>2.548</v>
       </c>
       <c r="D210" s="5">
         <f t="shared" ref="D210:D211" si="117">(C210-B210)/2</f>
-        <v>6.1000000000000165E-2</v>
+        <v>6.0999999999999943E-2</v>
       </c>
       <c r="E210" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F210" s="5">
         <f t="shared" ref="F210:F211" si="118">C210+E210</f>
-        <v>2.5580000000000003</v>
+        <v>2.5510000000000002</v>
       </c>
       <c r="G210" s="5">
         <f t="shared" ref="G210:G211" si="119">B210-E210</f>
-        <v>2.4299999999999997</v>
+        <v>2.423</v>
       </c>
       <c r="H210" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="I210" s="6" t="s">
         <v>179</v>
@@ -5885,31 +6186,31 @@
     </row>
     <row r="211" spans="1:9">
       <c r="A211" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B211" s="5">
-        <v>2.875</v>
+        <v>2.8679999999999999</v>
       </c>
       <c r="C211" s="5">
-        <v>2.9969999999999999</v>
+        <v>2.99</v>
       </c>
       <c r="D211" s="5">
         <f t="shared" si="117"/>
-        <v>6.0999999999999943E-2</v>
+        <v>6.1000000000000165E-2</v>
       </c>
       <c r="E211" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F211" s="5">
         <f t="shared" si="118"/>
-        <v>3</v>
+        <v>2.9930000000000003</v>
       </c>
       <c r="G211" s="5">
         <f t="shared" si="119"/>
-        <v>2.8719999999999999</v>
+        <v>2.8649999999999998</v>
       </c>
       <c r="H211" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="I211" s="6" t="s">
         <v>179</v>
@@ -5917,13 +6218,13 @@
     </row>
     <row r="212" spans="1:9">
       <c r="A212" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B212" s="5">
-        <v>3.6669999999999998</v>
+        <v>3.66</v>
       </c>
       <c r="C212" s="5">
-        <v>3.8969999999999998</v>
+        <v>3.89</v>
       </c>
       <c r="D212" s="5">
         <f t="shared" ref="D212" si="120">(C212-B212)/2</f>
@@ -5934,17 +6235,510 @@
       </c>
       <c r="F212" s="5">
         <f t="shared" ref="F212" si="121">C212+E212</f>
-        <v>3.9</v>
+        <v>3.8930000000000002</v>
       </c>
       <c r="G212" s="5">
         <f t="shared" ref="G212" si="122">B212-E212</f>
-        <v>3.6639999999999997</v>
+        <v>3.657</v>
       </c>
       <c r="H212" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="I212" s="6" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9">
+      <c r="A216" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9">
+      <c r="A218" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9">
+      <c r="A220" t="s">
+        <v>241</v>
+      </c>
+      <c r="B220" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C220" s="5">
+        <v>1</v>
+      </c>
+      <c r="D220" s="5">
+        <f t="shared" ref="D220" si="123">(C220-B220)/2</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="E220" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F220" s="5">
+        <f t="shared" ref="F220" si="124">C220+E220</f>
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="G220" s="5">
+        <f t="shared" ref="G220" si="125">B220-E220</f>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="H220" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9">
+      <c r="A221" t="s">
+        <v>240</v>
+      </c>
+      <c r="B221" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C221" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="D221" s="5">
+        <f t="shared" ref="D221" si="126">(C221-B221)/2</f>
+        <v>3.5000000000000031E-2</v>
+      </c>
+      <c r="E221" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F221" s="5">
+        <f t="shared" ref="F221" si="127">C221+E221</f>
+        <v>1.2129999999999999</v>
+      </c>
+      <c r="G221" s="5">
+        <f t="shared" ref="G221" si="128">B221-E221</f>
+        <v>1.137</v>
+      </c>
+      <c r="H221" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9">
+      <c r="A222" t="s">
+        <v>237</v>
+      </c>
+      <c r="B222" s="5">
+        <v>1.52</v>
+      </c>
+      <c r="C222" s="5">
+        <v>1.63</v>
+      </c>
+      <c r="D222" s="5">
+        <f t="shared" ref="D222" si="129">(C222-B222)/2</f>
+        <v>5.4999999999999938E-2</v>
+      </c>
+      <c r="E222" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F222" s="5">
+        <f t="shared" ref="F222" si="130">C222+E222</f>
+        <v>1.6329999999999998</v>
+      </c>
+      <c r="G222" s="5">
+        <f t="shared" ref="G222" si="131">B222-E222</f>
+        <v>1.5170000000000001</v>
+      </c>
+      <c r="H222" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9">
+      <c r="A223" t="s">
+        <v>242</v>
+      </c>
+      <c r="I223" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9">
+      <c r="A224" t="s">
+        <v>243</v>
+      </c>
+      <c r="B224" s="5">
+        <v>2.14</v>
+      </c>
+      <c r="C224" s="5">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D224" s="5">
+        <f t="shared" ref="D224" si="132">(C224-B224)/2</f>
+        <v>5.9999999999999831E-2</v>
+      </c>
+      <c r="E224" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F224" s="5">
+        <f t="shared" ref="F224" si="133">C224+E224</f>
+        <v>2.2629999999999999</v>
+      </c>
+      <c r="G224" s="5">
+        <f t="shared" ref="G224" si="134">B224-E224</f>
+        <v>2.137</v>
+      </c>
+      <c r="H224" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9">
+      <c r="A225" t="s">
+        <v>244</v>
+      </c>
+      <c r="B225" s="5">
+        <v>2.56</v>
+      </c>
+      <c r="C225" s="5">
+        <v>2.63</v>
+      </c>
+      <c r="D225" s="5">
+        <f t="shared" ref="D225" si="135">(C225-B225)/2</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="E225" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F225" s="5">
+        <f t="shared" ref="F225" si="136">C225+E225</f>
+        <v>2.633</v>
+      </c>
+      <c r="G225" s="5">
+        <f t="shared" ref="G225" si="137">B225-E225</f>
+        <v>2.5569999999999999</v>
+      </c>
+      <c r="H225" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9">
+      <c r="A226" t="s">
+        <v>245</v>
+      </c>
+      <c r="B226" s="5">
+        <v>3</v>
+      </c>
+      <c r="C226" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="D226" s="5">
+        <f t="shared" ref="D226" si="138">(C226-B226)/2</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="E226" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F226" s="5">
+        <f t="shared" ref="F226" si="139">C226+E226</f>
+        <v>3.1030000000000002</v>
+      </c>
+      <c r="G226" s="5">
+        <f t="shared" ref="G226" si="140">B226-E226</f>
+        <v>2.9969999999999999</v>
+      </c>
+      <c r="H226" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9">
+      <c r="A227" t="s">
+        <v>246</v>
+      </c>
+      <c r="B227" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="C227" s="5">
+        <v>4</v>
+      </c>
+      <c r="D227" s="5">
+        <f t="shared" ref="D227" si="141">(C227-B227)/2</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="E227" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F227" s="5">
+        <f t="shared" ref="F227" si="142">C227+E227</f>
+        <v>4.0030000000000001</v>
+      </c>
+      <c r="G227" s="5">
+        <f t="shared" ref="G227" si="143">B227-E227</f>
+        <v>3.8969999999999998</v>
+      </c>
+      <c r="H227" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9">
+      <c r="A228" t="s">
+        <v>253</v>
+      </c>
+      <c r="B228" s="5">
+        <v>5.38</v>
+      </c>
+      <c r="C228" s="5">
+        <v>5.54</v>
+      </c>
+      <c r="D228" s="5">
+        <f t="shared" ref="D228" si="144">(C228-B228)/2</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="E228" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F228" s="5">
+        <f t="shared" ref="F228" si="145">C228+E228</f>
+        <v>5.5430000000000001</v>
+      </c>
+      <c r="G228" s="5">
+        <f t="shared" ref="G228" si="146">B228-E228</f>
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="H228" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9">
+      <c r="A230" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9">
+      <c r="A232" t="s">
+        <v>231</v>
+      </c>
+      <c r="B232" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="C232" s="5">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="D232" s="5">
+        <f t="shared" ref="D232" si="147">(C232-B232)/2</f>
+        <v>3.4999999999999976E-2</v>
+      </c>
+      <c r="E232" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F232" s="5">
+        <f t="shared" ref="F232" si="148">C232+E232</f>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="G232" s="5">
+        <f t="shared" ref="G232" si="149">B232-E232</f>
+        <v>0.872</v>
+      </c>
+      <c r="H232" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9">
+      <c r="A233" t="s">
+        <v>230</v>
+      </c>
+      <c r="B233" s="5">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="C233" s="5">
+        <v>1.135</v>
+      </c>
+      <c r="D233" s="5">
+        <f t="shared" ref="D233" si="150">(C233-B233)/2</f>
+        <v>3.5000000000000031E-2</v>
+      </c>
+      <c r="E233" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F233" s="5">
+        <f t="shared" ref="F233" si="151">C233+E233</f>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="G233" s="5">
+        <f t="shared" ref="G233" si="152">B233-E233</f>
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="H233" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9">
+      <c r="A234" t="s">
+        <v>229</v>
+      </c>
+      <c r="B234" s="5">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="C234" s="5">
+        <v>1.51</v>
+      </c>
+      <c r="D234" s="5">
+        <f t="shared" ref="D234" si="153">(C234-B234)/2</f>
+        <v>3.7499999999999978E-2</v>
+      </c>
+      <c r="E234" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F234" s="5">
+        <f t="shared" ref="F234" si="154">C234+E234</f>
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="G234" s="5">
+        <f t="shared" ref="G234" si="155">B234-E234</f>
+        <v>1.4320000000000002</v>
+      </c>
+      <c r="H234" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9">
+      <c r="A235" t="s">
+        <v>232</v>
+      </c>
+      <c r="B235" s="5">
+        <v>1.71</v>
+      </c>
+      <c r="C235" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="D235" s="5">
+        <f t="shared" ref="D235" si="156">(C235-B235)/2</f>
+        <v>4.500000000000004E-2</v>
+      </c>
+      <c r="E235" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F235" s="5">
+        <f t="shared" ref="F235" si="157">C235+E235</f>
+        <v>1.8029999999999999</v>
+      </c>
+      <c r="G235" s="5">
+        <f t="shared" ref="G235" si="158">B235-E235</f>
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="H235" t="s">
+        <v>233</v>
+      </c>
+      <c r="I235" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9">
+      <c r="A236" t="s">
+        <v>236</v>
+      </c>
+      <c r="B236" s="5">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="C236" s="5">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="D236" s="5">
+        <f t="shared" ref="D236" si="159">(C236-B236)/2</f>
+        <v>5.9999999999999831E-2</v>
+      </c>
+      <c r="E236" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F236" s="5">
+        <f t="shared" ref="F236" si="160">C236+E236</f>
+        <v>2.1379999999999999</v>
+      </c>
+      <c r="G236" s="5">
+        <f t="shared" ref="G236" si="161">B236-E236</f>
+        <v>2.012</v>
+      </c>
+      <c r="H236" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9">
+      <c r="A237" t="s">
+        <v>131</v>
+      </c>
+      <c r="B237" s="5">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="C237" s="5">
+        <v>2.6150000000000002</v>
+      </c>
+      <c r="D237" s="5">
+        <f t="shared" ref="D237" si="162">(C237-B237)/2</f>
+        <v>3.5000000000000142E-2</v>
+      </c>
+      <c r="E237" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F237" s="5">
+        <f t="shared" ref="F237" si="163">C237+E237</f>
+        <v>2.6180000000000003</v>
+      </c>
+      <c r="G237" s="5">
+        <f t="shared" ref="G237" si="164">B237-E237</f>
+        <v>2.5419999999999998</v>
+      </c>
+      <c r="H237" t="s">
+        <v>234</v>
+      </c>
+      <c r="I237" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="A238" t="s">
+        <v>132</v>
+      </c>
+      <c r="B238" s="5">
+        <v>2.8849999999999998</v>
+      </c>
+      <c r="C238" s="5">
+        <v>2.9950000000000001</v>
+      </c>
+      <c r="D238" s="5">
+        <f t="shared" ref="D238" si="165">(C238-B238)/2</f>
+        <v>5.500000000000016E-2</v>
+      </c>
+      <c r="E238" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F238" s="5">
+        <f t="shared" ref="F238" si="166">C238+E238</f>
+        <v>2.9980000000000002</v>
+      </c>
+      <c r="G238" s="5">
+        <f t="shared" ref="G238" si="167">B238-E238</f>
+        <v>2.8819999999999997</v>
+      </c>
+      <c r="H238" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9">
+      <c r="A239" t="s">
+        <v>235</v>
+      </c>
+      <c r="B239" s="5">
+        <v>3.7850000000000001</v>
+      </c>
+      <c r="C239" s="5">
+        <v>3.895</v>
+      </c>
+      <c r="D239" s="5">
+        <f t="shared" ref="D239" si="168">(C239-B239)/2</f>
+        <v>5.4999999999999938E-2</v>
+      </c>
+      <c r="E239" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F239" s="5">
+        <f t="shared" ref="F239" si="169">C239+E239</f>
+        <v>3.8980000000000001</v>
+      </c>
+      <c r="G239" s="5">
+        <f t="shared" ref="G239" si="170">B239-E239</f>
+        <v>3.782</v>
+      </c>
+      <c r="H239" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use formulas for tubes pinned to dimensions of other tubes
</commit_message>
<xml_diff>
--- a/data/body_tube_data.xlsx
+++ b/data/body_tube_data.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="288">
   <si>
     <t>ID inches</t>
   </si>
@@ -914,6 +914,33 @@
   </si>
   <si>
     <t>large clearance 0.013, is this right?</t>
+  </si>
+  <si>
+    <t>Carbon Fiber Airframes</t>
+  </si>
+  <si>
+    <t>FWCF-29</t>
+  </si>
+  <si>
+    <t>weight 1.8 oz/ft</t>
+  </si>
+  <si>
+    <t>FWCF-38</t>
+  </si>
+  <si>
+    <t>dimensions assumed same as FT16-STD</t>
+  </si>
+  <si>
+    <t>FWCF-54</t>
+  </si>
+  <si>
+    <t>dimensions assumed same as FT22-STD</t>
+  </si>
+  <si>
+    <t>FWCF-3</t>
+  </si>
+  <si>
+    <t>dimensions assumed same as FT30-STD</t>
   </si>
 </sst>
 </file>
@@ -1010,9 +1037,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="254">
+  <cellStyleXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1285,7 +1328,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="254">
+  <cellStyles count="270">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1412,6 +1455,14 @@
     <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1539,6 +1590,14 @@
     <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1868,12 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M239"/>
+  <dimension ref="A1:M247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <pane ySplit="5060" topLeftCell="A216"/>
-      <selection activeCell="A130" sqref="A130"/>
-      <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5870,874 +5927,1015 @@
         <v>179</v>
       </c>
     </row>
+    <row r="194" spans="1:9">
+      <c r="I194" s="6"/>
+    </row>
     <row r="195" spans="1:9">
       <c r="A195" s="1" t="s">
-        <v>212</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="I195" s="6"/>
+    </row>
+    <row r="196" spans="1:9">
+      <c r="I196" s="6"/>
     </row>
     <row r="197" spans="1:9">
       <c r="A197" t="s">
-        <v>213</v>
+        <v>280</v>
       </c>
       <c r="B197" s="5">
-        <v>1.1399999999999999</v>
+        <v>1.145</v>
       </c>
       <c r="C197" s="5">
-        <v>1.2150000000000001</v>
+        <v>1.2549999999999999</v>
       </c>
       <c r="D197" s="5">
-        <f t="shared" ref="D197:D204" si="108">(C197-B197)/2</f>
-        <v>3.7500000000000089E-2</v>
+        <f t="shared" ref="D197" si="108">(C197-B197)/2</f>
+        <v>5.4999999999999938E-2</v>
       </c>
       <c r="E197" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F197" s="5">
-        <f t="shared" ref="F197:F204" si="109">C197+E197</f>
-        <v>1.218</v>
+        <f t="shared" ref="F197" si="109">C197+E197</f>
+        <v>1.2579999999999998</v>
       </c>
       <c r="G197" s="5">
-        <f t="shared" ref="G197:G204" si="110">B197-E197</f>
-        <v>1.137</v>
-      </c>
+        <f t="shared" ref="G197" si="110">B197-E197</f>
+        <v>1.1420000000000001</v>
+      </c>
+      <c r="H197" t="s">
+        <v>281</v>
+      </c>
+      <c r="I197" s="6"/>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" t="s">
-        <v>214</v>
+        <v>282</v>
       </c>
       <c r="B198" s="5">
-        <v>1.5249999999999999</v>
+        <v>1.52</v>
       </c>
       <c r="C198" s="5">
-        <v>1.61</v>
+        <v>1.645</v>
       </c>
       <c r="D198" s="5">
-        <f t="shared" si="108"/>
-        <v>4.2500000000000093E-2</v>
+        <f t="shared" ref="D198" si="111">(C198-B198)/2</f>
+        <v>6.25E-2</v>
       </c>
       <c r="E198" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F198" s="5">
-        <f t="shared" si="109"/>
-        <v>1.613</v>
+        <f t="shared" ref="F198" si="112">C198+E198</f>
+        <v>1.6479999999999999</v>
       </c>
       <c r="G198" s="5">
-        <f t="shared" si="110"/>
-        <v>1.522</v>
+        <f t="shared" ref="G198" si="113">B198-E198</f>
+        <v>1.5170000000000001</v>
+      </c>
+      <c r="H198" t="s">
+        <v>283</v>
+      </c>
+      <c r="I198" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" t="s">
-        <v>215</v>
+        <v>284</v>
       </c>
       <c r="B199" s="5">
-        <v>1.5249999999999999</v>
+        <v>2.1520000000000001</v>
       </c>
       <c r="C199" s="5">
-        <v>1.635</v>
+        <v>2.2770000000000001</v>
       </c>
       <c r="D199" s="5">
-        <f t="shared" si="108"/>
-        <v>5.5000000000000049E-2</v>
+        <f t="shared" ref="D199" si="114">(C199-B199)/2</f>
+        <v>6.25E-2</v>
       </c>
       <c r="E199" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F199" s="5">
-        <f t="shared" si="109"/>
-        <v>1.6379999999999999</v>
+        <f t="shared" ref="F199" si="115">C199+E199</f>
+        <v>2.2800000000000002</v>
       </c>
       <c r="G199" s="5">
-        <f t="shared" si="110"/>
-        <v>1.522</v>
+        <f t="shared" ref="G199" si="116">B199-E199</f>
+        <v>2.149</v>
+      </c>
+      <c r="H199" t="s">
+        <v>285</v>
+      </c>
+      <c r="I199" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="200" spans="1:9">
       <c r="A200" t="s">
-        <v>216</v>
+        <v>286</v>
       </c>
       <c r="B200" s="5">
-        <v>2.14</v>
+        <v>3</v>
       </c>
       <c r="C200" s="5">
-        <v>2.2599999999999998</v>
+        <v>3.125</v>
       </c>
       <c r="D200" s="5">
-        <f t="shared" si="108"/>
-        <v>5.9999999999999831E-2</v>
+        <f t="shared" ref="D200" si="117">(C200-B200)/2</f>
+        <v>6.25E-2</v>
       </c>
       <c r="E200" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F200" s="5">
-        <f t="shared" si="109"/>
-        <v>2.2629999999999999</v>
+        <f t="shared" ref="F200" si="118">C200+E200</f>
+        <v>3.1280000000000001</v>
       </c>
       <c r="G200" s="5">
-        <f t="shared" si="110"/>
-        <v>2.137</v>
+        <f t="shared" ref="G200" si="119">B200-E200</f>
+        <v>2.9969999999999999</v>
+      </c>
+      <c r="H200" t="s">
+        <v>287</v>
+      </c>
+      <c r="I200" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="201" spans="1:9">
-      <c r="A201" t="s">
-        <v>217</v>
-      </c>
-      <c r="B201" s="5">
-        <v>2.1749999999999998</v>
-      </c>
-      <c r="C201" s="5">
-        <v>2.2450000000000001</v>
-      </c>
-      <c r="D201" s="5">
-        <f t="shared" si="108"/>
-        <v>3.5000000000000142E-2</v>
-      </c>
-      <c r="E201" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F201" s="5">
-        <f t="shared" si="109"/>
-        <v>2.2480000000000002</v>
-      </c>
-      <c r="G201" s="5">
-        <f t="shared" si="110"/>
-        <v>2.1719999999999997</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9">
-      <c r="A202" t="s">
-        <v>218</v>
-      </c>
-      <c r="B202" s="5">
-        <v>2.5579999999999998</v>
-      </c>
-      <c r="C202" s="5">
-        <v>2.64</v>
-      </c>
-      <c r="D202" s="5">
-        <f t="shared" si="108"/>
-        <v>4.1000000000000147E-2</v>
-      </c>
-      <c r="E202" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F202" s="5">
-        <f t="shared" si="109"/>
-        <v>2.6430000000000002</v>
-      </c>
-      <c r="G202" s="5">
-        <f t="shared" si="110"/>
-        <v>2.5549999999999997</v>
-      </c>
+      <c r="I201" s="6"/>
     </row>
     <row r="203" spans="1:9">
-      <c r="A203" t="s">
-        <v>219</v>
-      </c>
-      <c r="B203" s="5">
-        <v>3</v>
-      </c>
-      <c r="C203" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="D203" s="5">
-        <f t="shared" si="108"/>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="E203" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F203" s="5">
-        <f t="shared" si="109"/>
-        <v>3.1030000000000002</v>
-      </c>
-      <c r="G203" s="5">
-        <f t="shared" si="110"/>
-        <v>2.9969999999999999</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9">
-      <c r="A204" t="s">
-        <v>220</v>
-      </c>
-      <c r="B204" s="5">
-        <v>3.9</v>
-      </c>
-      <c r="C204" s="5">
-        <v>4</v>
-      </c>
-      <c r="D204" s="5">
-        <f t="shared" si="108"/>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="E204" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F204" s="5">
-        <f t="shared" si="109"/>
-        <v>4.0030000000000001</v>
-      </c>
-      <c r="G204" s="5">
-        <f t="shared" si="110"/>
-        <v>3.8969999999999998</v>
+      <c r="A203" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9">
+      <c r="A205" t="s">
+        <v>213</v>
+      </c>
+      <c r="B205" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C205" s="5">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="D205" s="5">
+        <f t="shared" ref="D205:D212" si="120">(C205-B205)/2</f>
+        <v>3.7500000000000089E-2</v>
+      </c>
+      <c r="E205" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F205" s="5">
+        <f t="shared" ref="F205:F212" si="121">C205+E205</f>
+        <v>1.218</v>
+      </c>
+      <c r="G205" s="5">
+        <f t="shared" ref="G205:G212" si="122">B205-E205</f>
+        <v>1.137</v>
       </c>
     </row>
     <row r="206" spans="1:9">
-      <c r="A206" s="1" t="s">
-        <v>221</v>
+      <c r="A206" t="s">
+        <v>214</v>
+      </c>
+      <c r="B206" s="5">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="C206" s="5">
+        <v>1.61</v>
+      </c>
+      <c r="D206" s="5">
+        <f t="shared" si="120"/>
+        <v>4.2500000000000093E-2</v>
+      </c>
+      <c r="E206" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F206" s="5">
+        <f t="shared" si="121"/>
+        <v>1.613</v>
+      </c>
+      <c r="G206" s="5">
+        <f t="shared" si="122"/>
+        <v>1.522</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9">
+      <c r="A207" t="s">
+        <v>215</v>
+      </c>
+      <c r="B207" s="5">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="C207" s="5">
+        <v>1.635</v>
+      </c>
+      <c r="D207" s="5">
+        <f t="shared" si="120"/>
+        <v>5.5000000000000049E-2</v>
+      </c>
+      <c r="E207" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F207" s="5">
+        <f t="shared" si="121"/>
+        <v>1.6379999999999999</v>
+      </c>
+      <c r="G207" s="5">
+        <f t="shared" si="122"/>
+        <v>1.522</v>
       </c>
     </row>
     <row r="208" spans="1:9">
       <c r="A208" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B208" s="5">
-        <v>1.393</v>
+        <v>2.14</v>
       </c>
       <c r="C208" s="5">
-        <v>1.5149999999999999</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D208" s="5">
-        <f t="shared" ref="D208" si="111">(C208-B208)/2</f>
-        <v>6.0999999999999943E-2</v>
+        <f t="shared" si="120"/>
+        <v>5.9999999999999831E-2</v>
       </c>
       <c r="E208" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F208" s="5">
-        <f t="shared" ref="F208" si="112">C208+E208</f>
-        <v>1.5179999999999998</v>
+        <f t="shared" si="121"/>
+        <v>2.2629999999999999</v>
       </c>
       <c r="G208" s="5">
-        <f t="shared" ref="G208" si="113">B208-E208</f>
-        <v>1.3900000000000001</v>
-      </c>
-      <c r="H208" t="s">
-        <v>238</v>
-      </c>
-      <c r="I208" s="6" t="s">
-        <v>179</v>
+        <f t="shared" si="122"/>
+        <v>2.137</v>
       </c>
     </row>
     <row r="209" spans="1:9">
       <c r="A209" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B209" s="5">
-        <v>2.0430000000000001</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="C209" s="5">
-        <v>2.165</v>
+        <v>2.2450000000000001</v>
       </c>
       <c r="D209" s="5">
-        <f t="shared" ref="D209" si="114">(C209-B209)/2</f>
-        <v>6.0999999999999943E-2</v>
+        <f t="shared" si="120"/>
+        <v>3.5000000000000142E-2</v>
       </c>
       <c r="E209" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F209" s="5">
-        <f t="shared" ref="F209" si="115">C209+E209</f>
-        <v>2.1680000000000001</v>
+        <f t="shared" si="121"/>
+        <v>2.2480000000000002</v>
       </c>
       <c r="G209" s="5">
-        <f t="shared" ref="G209" si="116">B209-E209</f>
-        <v>2.04</v>
-      </c>
-      <c r="H209" t="s">
-        <v>238</v>
-      </c>
-      <c r="I209" s="6" t="s">
-        <v>179</v>
+        <f t="shared" si="122"/>
+        <v>2.1719999999999997</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B210" s="5">
-        <v>2.4260000000000002</v>
+        <v>2.5579999999999998</v>
       </c>
       <c r="C210" s="5">
-        <v>2.548</v>
+        <v>2.64</v>
       </c>
       <c r="D210" s="5">
-        <f t="shared" ref="D210:D211" si="117">(C210-B210)/2</f>
-        <v>6.0999999999999943E-2</v>
+        <f t="shared" si="120"/>
+        <v>4.1000000000000147E-2</v>
       </c>
       <c r="E210" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F210" s="5">
-        <f t="shared" ref="F210:F211" si="118">C210+E210</f>
-        <v>2.5510000000000002</v>
+        <f t="shared" si="121"/>
+        <v>2.6430000000000002</v>
       </c>
       <c r="G210" s="5">
-        <f t="shared" ref="G210:G211" si="119">B210-E210</f>
-        <v>2.423</v>
-      </c>
-      <c r="H210" t="s">
-        <v>238</v>
-      </c>
-      <c r="I210" s="6" t="s">
-        <v>179</v>
+        <f t="shared" si="122"/>
+        <v>2.5549999999999997</v>
       </c>
     </row>
     <row r="211" spans="1:9">
       <c r="A211" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B211" s="5">
-        <v>2.8679999999999999</v>
+        <v>3</v>
       </c>
       <c r="C211" s="5">
-        <v>2.99</v>
+        <v>3.1</v>
       </c>
       <c r="D211" s="5">
-        <f t="shared" si="117"/>
-        <v>6.1000000000000165E-2</v>
+        <f t="shared" si="120"/>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="E211" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F211" s="5">
-        <f t="shared" si="118"/>
-        <v>2.9930000000000003</v>
+        <f t="shared" si="121"/>
+        <v>3.1030000000000002</v>
       </c>
       <c r="G211" s="5">
-        <f t="shared" si="119"/>
-        <v>2.8649999999999998</v>
-      </c>
-      <c r="H211" t="s">
-        <v>238</v>
-      </c>
-      <c r="I211" s="6" t="s">
-        <v>179</v>
+        <f t="shared" si="122"/>
+        <v>2.9969999999999999</v>
       </c>
     </row>
     <row r="212" spans="1:9">
       <c r="A212" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B212" s="5">
-        <v>3.66</v>
+        <v>3.9</v>
       </c>
       <c r="C212" s="5">
-        <v>3.89</v>
+        <v>4</v>
       </c>
       <c r="D212" s="5">
-        <f t="shared" ref="D212" si="120">(C212-B212)/2</f>
-        <v>0.11499999999999999</v>
+        <f t="shared" si="120"/>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="E212" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F212" s="5">
-        <f t="shared" ref="F212" si="121">C212+E212</f>
-        <v>3.8930000000000002</v>
+        <f t="shared" si="121"/>
+        <v>4.0030000000000001</v>
       </c>
       <c r="G212" s="5">
-        <f t="shared" ref="G212" si="122">B212-E212</f>
-        <v>3.657</v>
-      </c>
-      <c r="H212" t="s">
-        <v>239</v>
-      </c>
-      <c r="I212" s="6" t="s">
+        <f t="shared" si="122"/>
+        <v>3.8969999999999998</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9">
+      <c r="A214" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9">
+      <c r="A216" t="s">
+        <v>222</v>
+      </c>
+      <c r="B216" s="5">
+        <v>1.393</v>
+      </c>
+      <c r="C216" s="5">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="D216" s="5">
+        <f t="shared" ref="D216" si="123">(C216-B216)/2</f>
+        <v>6.0999999999999943E-2</v>
+      </c>
+      <c r="E216" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F216" s="5">
+        <f t="shared" ref="F216" si="124">C216+E216</f>
+        <v>1.5179999999999998</v>
+      </c>
+      <c r="G216" s="5">
+        <f t="shared" ref="G216" si="125">B216-E216</f>
+        <v>1.3900000000000001</v>
+      </c>
+      <c r="H216" t="s">
+        <v>238</v>
+      </c>
+      <c r="I216" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
-      <c r="A216" s="1" t="s">
-        <v>228</v>
+    <row r="217" spans="1:9">
+      <c r="A217" t="s">
+        <v>223</v>
+      </c>
+      <c r="B217" s="5">
+        <v>2.0430000000000001</v>
+      </c>
+      <c r="C217" s="5">
+        <v>2.165</v>
+      </c>
+      <c r="D217" s="5">
+        <f t="shared" ref="D217" si="126">(C217-B217)/2</f>
+        <v>6.0999999999999943E-2</v>
+      </c>
+      <c r="E217" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F217" s="5">
+        <f t="shared" ref="F217" si="127">C217+E217</f>
+        <v>2.1680000000000001</v>
+      </c>
+      <c r="G217" s="5">
+        <f t="shared" ref="G217" si="128">B217-E217</f>
+        <v>2.04</v>
+      </c>
+      <c r="H217" t="s">
+        <v>238</v>
+      </c>
+      <c r="I217" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="218" spans="1:9">
-      <c r="A218" s="1" t="s">
-        <v>257</v>
+      <c r="A218" t="s">
+        <v>224</v>
+      </c>
+      <c r="B218" s="5">
+        <v>2.4260000000000002</v>
+      </c>
+      <c r="C218" s="5">
+        <v>2.548</v>
+      </c>
+      <c r="D218" s="5">
+        <f t="shared" ref="D218:D219" si="129">(C218-B218)/2</f>
+        <v>6.0999999999999943E-2</v>
+      </c>
+      <c r="E218" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F218" s="5">
+        <f t="shared" ref="F218:F219" si="130">C218+E218</f>
+        <v>2.5510000000000002</v>
+      </c>
+      <c r="G218" s="5">
+        <f t="shared" ref="G218:G219" si="131">B218-E218</f>
+        <v>2.423</v>
+      </c>
+      <c r="H218" t="s">
+        <v>238</v>
+      </c>
+      <c r="I218" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9">
+      <c r="A219" t="s">
+        <v>225</v>
+      </c>
+      <c r="B219" s="5">
+        <v>2.8679999999999999</v>
+      </c>
+      <c r="C219" s="5">
+        <v>2.99</v>
+      </c>
+      <c r="D219" s="5">
+        <f t="shared" si="129"/>
+        <v>6.1000000000000165E-2</v>
+      </c>
+      <c r="E219" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F219" s="5">
+        <f t="shared" si="130"/>
+        <v>2.9930000000000003</v>
+      </c>
+      <c r="G219" s="5">
+        <f t="shared" si="131"/>
+        <v>2.8649999999999998</v>
+      </c>
+      <c r="H219" t="s">
+        <v>238</v>
+      </c>
+      <c r="I219" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="220" spans="1:9">
       <c r="A220" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B220" s="5">
-        <v>0.95</v>
+        <v>3.66</v>
       </c>
       <c r="C220" s="5">
-        <v>1</v>
+        <v>3.89</v>
       </c>
       <c r="D220" s="5">
-        <f t="shared" ref="D220" si="123">(C220-B220)/2</f>
-        <v>2.5000000000000022E-2</v>
+        <f t="shared" ref="D220" si="132">(C220-B220)/2</f>
+        <v>0.11499999999999999</v>
       </c>
       <c r="E220" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F220" s="5">
-        <f t="shared" ref="F220" si="124">C220+E220</f>
-        <v>1.0029999999999999</v>
+        <f t="shared" ref="F220" si="133">C220+E220</f>
+        <v>3.8930000000000002</v>
       </c>
       <c r="G220" s="5">
-        <f t="shared" ref="G220" si="125">B220-E220</f>
-        <v>0.94699999999999995</v>
+        <f t="shared" ref="G220" si="134">B220-E220</f>
+        <v>3.657</v>
       </c>
       <c r="H220" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9">
-      <c r="A221" t="s">
-        <v>240</v>
-      </c>
-      <c r="B221" s="5">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="C221" s="5">
-        <v>1.21</v>
-      </c>
-      <c r="D221" s="5">
-        <f t="shared" ref="D221" si="126">(C221-B221)/2</f>
-        <v>3.5000000000000031E-2</v>
-      </c>
-      <c r="E221" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F221" s="5">
-        <f t="shared" ref="F221" si="127">C221+E221</f>
-        <v>1.2129999999999999</v>
-      </c>
-      <c r="G221" s="5">
-        <f t="shared" ref="G221" si="128">B221-E221</f>
-        <v>1.137</v>
-      </c>
-      <c r="H221" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="222" spans="1:9">
-      <c r="A222" t="s">
-        <v>237</v>
-      </c>
-      <c r="B222" s="5">
-        <v>1.52</v>
-      </c>
-      <c r="C222" s="5">
-        <v>1.63</v>
-      </c>
-      <c r="D222" s="5">
-        <f t="shared" ref="D222" si="129">(C222-B222)/2</f>
-        <v>5.4999999999999938E-2</v>
-      </c>
-      <c r="E222" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F222" s="5">
-        <f t="shared" ref="F222" si="130">C222+E222</f>
-        <v>1.6329999999999998</v>
-      </c>
-      <c r="G222" s="5">
-        <f t="shared" ref="G222" si="131">B222-E222</f>
-        <v>1.5170000000000001</v>
-      </c>
-      <c r="H222" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="223" spans="1:9">
-      <c r="A223" t="s">
-        <v>242</v>
-      </c>
-      <c r="I223" t="s">
-        <v>256</v>
+        <v>239</v>
+      </c>
+      <c r="I220" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="224" spans="1:9">
-      <c r="A224" t="s">
-        <v>243</v>
-      </c>
-      <c r="B224" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="C224" s="5">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="D224" s="5">
-        <f t="shared" ref="D224" si="132">(C224-B224)/2</f>
-        <v>5.9999999999999831E-2</v>
-      </c>
-      <c r="E224" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F224" s="5">
-        <f t="shared" ref="F224" si="133">C224+E224</f>
-        <v>2.2629999999999999</v>
-      </c>
-      <c r="G224" s="5">
-        <f t="shared" ref="G224" si="134">B224-E224</f>
-        <v>2.137</v>
-      </c>
-      <c r="H224" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9">
-      <c r="A225" t="s">
-        <v>244</v>
-      </c>
-      <c r="B225" s="5">
-        <v>2.56</v>
-      </c>
-      <c r="C225" s="5">
-        <v>2.63</v>
-      </c>
-      <c r="D225" s="5">
-        <f t="shared" ref="D225" si="135">(C225-B225)/2</f>
-        <v>3.499999999999992E-2</v>
-      </c>
-      <c r="E225" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F225" s="5">
-        <f t="shared" ref="F225" si="136">C225+E225</f>
-        <v>2.633</v>
-      </c>
-      <c r="G225" s="5">
-        <f t="shared" ref="G225" si="137">B225-E225</f>
-        <v>2.5569999999999999</v>
-      </c>
-      <c r="H225" t="s">
-        <v>247</v>
+      <c r="A224" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:9">
-      <c r="A226" t="s">
-        <v>245</v>
-      </c>
-      <c r="B226" s="5">
-        <v>3</v>
-      </c>
-      <c r="C226" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="D226" s="5">
-        <f t="shared" ref="D226" si="138">(C226-B226)/2</f>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="E226" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F226" s="5">
-        <f t="shared" ref="F226" si="139">C226+E226</f>
-        <v>3.1030000000000002</v>
-      </c>
-      <c r="G226" s="5">
-        <f t="shared" ref="G226" si="140">B226-E226</f>
-        <v>2.9969999999999999</v>
-      </c>
-      <c r="H226" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9">
-      <c r="A227" t="s">
-        <v>246</v>
-      </c>
-      <c r="B227" s="5">
-        <v>3.9</v>
-      </c>
-      <c r="C227" s="5">
-        <v>4</v>
-      </c>
-      <c r="D227" s="5">
-        <f t="shared" ref="D227" si="141">(C227-B227)/2</f>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="E227" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F227" s="5">
-        <f t="shared" ref="F227" si="142">C227+E227</f>
-        <v>4.0030000000000001</v>
-      </c>
-      <c r="G227" s="5">
-        <f t="shared" ref="G227" si="143">B227-E227</f>
-        <v>3.8969999999999998</v>
-      </c>
-      <c r="H227" t="s">
-        <v>251</v>
+      <c r="A226" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="228" spans="1:9">
       <c r="A228" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B228" s="5">
-        <v>5.38</v>
+        <v>0.95</v>
       </c>
       <c r="C228" s="5">
-        <v>5.54</v>
+        <v>1</v>
       </c>
       <c r="D228" s="5">
-        <f t="shared" ref="D228" si="144">(C228-B228)/2</f>
-        <v>8.0000000000000071E-2</v>
+        <f t="shared" ref="D228" si="135">(C228-B228)/2</f>
+        <v>2.5000000000000022E-2</v>
       </c>
       <c r="E228" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F228" s="5">
-        <f t="shared" ref="F228" si="145">C228+E228</f>
-        <v>5.5430000000000001</v>
+        <f t="shared" ref="F228" si="136">C228+E228</f>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G228" s="5">
-        <f t="shared" ref="G228" si="146">B228-E228</f>
-        <v>5.3769999999999998</v>
+        <f t="shared" ref="G228" si="137">B228-E228</f>
+        <v>0.94699999999999995</v>
       </c>
       <c r="H228" t="s">
-        <v>254</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9">
+      <c r="A229" t="s">
+        <v>240</v>
+      </c>
+      <c r="B229" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C229" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="D229" s="5">
+        <f t="shared" ref="D229" si="138">(C229-B229)/2</f>
+        <v>3.5000000000000031E-2</v>
+      </c>
+      <c r="E229" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F229" s="5">
+        <f t="shared" ref="F229" si="139">C229+E229</f>
+        <v>1.2129999999999999</v>
+      </c>
+      <c r="G229" s="5">
+        <f t="shared" ref="G229" si="140">B229-E229</f>
+        <v>1.137</v>
+      </c>
+      <c r="H229" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="230" spans="1:9">
-      <c r="A230" s="1" t="s">
-        <v>258</v>
+      <c r="A230" t="s">
+        <v>237</v>
+      </c>
+      <c r="B230" s="5">
+        <v>1.52</v>
+      </c>
+      <c r="C230" s="5">
+        <v>1.63</v>
+      </c>
+      <c r="D230" s="5">
+        <f t="shared" ref="D230" si="141">(C230-B230)/2</f>
+        <v>5.4999999999999938E-2</v>
+      </c>
+      <c r="E230" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F230" s="5">
+        <f t="shared" ref="F230" si="142">C230+E230</f>
+        <v>1.6329999999999998</v>
+      </c>
+      <c r="G230" s="5">
+        <f t="shared" ref="G230" si="143">B230-E230</f>
+        <v>1.5170000000000001</v>
+      </c>
+      <c r="H230" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9">
+      <c r="A231" t="s">
+        <v>242</v>
+      </c>
+      <c r="I231" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="232" spans="1:9">
       <c r="A232" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B232" s="5">
-        <v>0.875</v>
+        <v>2.14</v>
       </c>
       <c r="C232" s="5">
-        <v>0.94499999999999995</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D232" s="5">
-        <f t="shared" ref="D232" si="147">(C232-B232)/2</f>
-        <v>3.4999999999999976E-2</v>
+        <f t="shared" ref="D232" si="144">(C232-B232)/2</f>
+        <v>5.9999999999999831E-2</v>
       </c>
       <c r="E232" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F232" s="5">
-        <f t="shared" ref="F232" si="148">C232+E232</f>
-        <v>0.94799999999999995</v>
+        <f t="shared" ref="F232" si="145">C232+E232</f>
+        <v>2.2629999999999999</v>
       </c>
       <c r="G232" s="5">
-        <f t="shared" ref="G232" si="149">B232-E232</f>
-        <v>0.872</v>
+        <f t="shared" ref="G232" si="146">B232-E232</f>
+        <v>2.137</v>
       </c>
       <c r="H232" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="233" spans="1:9">
       <c r="A233" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B233" s="5">
-        <v>1.0649999999999999</v>
+        <v>2.56</v>
       </c>
       <c r="C233" s="5">
-        <v>1.135</v>
+        <v>2.63</v>
       </c>
       <c r="D233" s="5">
-        <f t="shared" ref="D233" si="150">(C233-B233)/2</f>
-        <v>3.5000000000000031E-2</v>
+        <f t="shared" ref="D233" si="147">(C233-B233)/2</f>
+        <v>3.499999999999992E-2</v>
       </c>
       <c r="E233" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F233" s="5">
-        <f t="shared" ref="F233" si="151">C233+E233</f>
-        <v>1.1379999999999999</v>
+        <f t="shared" ref="F233" si="148">C233+E233</f>
+        <v>2.633</v>
       </c>
       <c r="G233" s="5">
-        <f t="shared" ref="G233" si="152">B233-E233</f>
-        <v>1.0620000000000001</v>
+        <f t="shared" ref="G233" si="149">B233-E233</f>
+        <v>2.5569999999999999</v>
       </c>
       <c r="H233" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="234" spans="1:9">
       <c r="A234" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="B234" s="5">
-        <v>1.4350000000000001</v>
+        <v>3</v>
       </c>
       <c r="C234" s="5">
-        <v>1.51</v>
+        <v>3.1</v>
       </c>
       <c r="D234" s="5">
-        <f t="shared" ref="D234" si="153">(C234-B234)/2</f>
-        <v>3.7499999999999978E-2</v>
+        <f t="shared" ref="D234" si="150">(C234-B234)/2</f>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="E234" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F234" s="5">
-        <f t="shared" ref="F234" si="154">C234+E234</f>
-        <v>1.5129999999999999</v>
+        <f t="shared" ref="F234" si="151">C234+E234</f>
+        <v>3.1030000000000002</v>
       </c>
       <c r="G234" s="5">
-        <f t="shared" ref="G234" si="155">B234-E234</f>
-        <v>1.4320000000000002</v>
+        <f t="shared" ref="G234" si="152">B234-E234</f>
+        <v>2.9969999999999999</v>
       </c>
       <c r="H234" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="235" spans="1:9">
       <c r="A235" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B235" s="5">
-        <v>1.71</v>
+        <v>3.9</v>
       </c>
       <c r="C235" s="5">
-        <v>1.8</v>
+        <v>4</v>
       </c>
       <c r="D235" s="5">
-        <f t="shared" ref="D235" si="156">(C235-B235)/2</f>
-        <v>4.500000000000004E-2</v>
+        <f t="shared" ref="D235" si="153">(C235-B235)/2</f>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="E235" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F235" s="5">
-        <f t="shared" ref="F235" si="157">C235+E235</f>
-        <v>1.8029999999999999</v>
+        <f t="shared" ref="F235" si="154">C235+E235</f>
+        <v>4.0030000000000001</v>
       </c>
       <c r="G235" s="5">
-        <f t="shared" ref="G235" si="158">B235-E235</f>
-        <v>1.7070000000000001</v>
+        <f t="shared" ref="G235" si="155">B235-E235</f>
+        <v>3.8969999999999998</v>
       </c>
       <c r="H235" t="s">
-        <v>233</v>
-      </c>
-      <c r="I235" s="4" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="236" spans="1:9">
       <c r="A236" t="s">
+        <v>253</v>
+      </c>
+      <c r="B236" s="5">
+        <v>5.38</v>
+      </c>
+      <c r="C236" s="5">
+        <v>5.54</v>
+      </c>
+      <c r="D236" s="5">
+        <f t="shared" ref="D236" si="156">(C236-B236)/2</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="E236" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F236" s="5">
+        <f t="shared" ref="F236" si="157">C236+E236</f>
+        <v>5.5430000000000001</v>
+      </c>
+      <c r="G236" s="5">
+        <f t="shared" ref="G236" si="158">B236-E236</f>
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="H236" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="A238" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9">
+      <c r="A240" t="s">
+        <v>231</v>
+      </c>
+      <c r="B240" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="C240" s="5">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="D240" s="5">
+        <f t="shared" ref="D240" si="159">(C240-B240)/2</f>
+        <v>3.4999999999999976E-2</v>
+      </c>
+      <c r="E240" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F240" s="5">
+        <f t="shared" ref="F240" si="160">C240+E240</f>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="G240" s="5">
+        <f t="shared" ref="G240" si="161">B240-E240</f>
+        <v>0.872</v>
+      </c>
+      <c r="H240" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9">
+      <c r="A241" t="s">
+        <v>230</v>
+      </c>
+      <c r="B241" s="5">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="C241" s="5">
+        <v>1.135</v>
+      </c>
+      <c r="D241" s="5">
+        <f t="shared" ref="D241" si="162">(C241-B241)/2</f>
+        <v>3.5000000000000031E-2</v>
+      </c>
+      <c r="E241" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F241" s="5">
+        <f t="shared" ref="F241" si="163">C241+E241</f>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="G241" s="5">
+        <f t="shared" ref="G241" si="164">B241-E241</f>
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="H241" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9">
+      <c r="A242" t="s">
+        <v>229</v>
+      </c>
+      <c r="B242" s="5">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="C242" s="5">
+        <v>1.51</v>
+      </c>
+      <c r="D242" s="5">
+        <f t="shared" ref="D242" si="165">(C242-B242)/2</f>
+        <v>3.7499999999999978E-2</v>
+      </c>
+      <c r="E242" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F242" s="5">
+        <f t="shared" ref="F242" si="166">C242+E242</f>
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="G242" s="5">
+        <f t="shared" ref="G242" si="167">B242-E242</f>
+        <v>1.4320000000000002</v>
+      </c>
+      <c r="H242" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9">
+      <c r="A243" t="s">
+        <v>232</v>
+      </c>
+      <c r="B243" s="5">
+        <v>1.71</v>
+      </c>
+      <c r="C243" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="D243" s="5">
+        <f t="shared" ref="D243" si="168">(C243-B243)/2</f>
+        <v>4.500000000000004E-2</v>
+      </c>
+      <c r="E243" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F243" s="5">
+        <f t="shared" ref="F243" si="169">C243+E243</f>
+        <v>1.8029999999999999</v>
+      </c>
+      <c r="G243" s="5">
+        <f t="shared" ref="G243" si="170">B243-E243</f>
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="H243" t="s">
+        <v>233</v>
+      </c>
+      <c r="I243" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9">
+      <c r="A244" t="s">
         <v>236</v>
       </c>
-      <c r="B236" s="5">
+      <c r="B244" s="5">
         <v>2.0150000000000001</v>
       </c>
-      <c r="C236" s="5">
+      <c r="C244" s="5">
         <v>2.1349999999999998</v>
       </c>
-      <c r="D236" s="5">
-        <f t="shared" ref="D236" si="159">(C236-B236)/2</f>
+      <c r="D244" s="5">
+        <f t="shared" ref="D244" si="171">(C244-B244)/2</f>
         <v>5.9999999999999831E-2</v>
       </c>
-      <c r="E236" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F236" s="5">
-        <f t="shared" ref="F236" si="160">C236+E236</f>
+      <c r="E244" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F244" s="5">
+        <f t="shared" ref="F244" si="172">C244+E244</f>
         <v>2.1379999999999999</v>
       </c>
-      <c r="G236" s="5">
-        <f t="shared" ref="G236" si="161">B236-E236</f>
+      <c r="G244" s="5">
+        <f t="shared" ref="G244" si="173">B244-E244</f>
         <v>2.012</v>
       </c>
-      <c r="H236" t="s">
+      <c r="H244" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
-      <c r="A237" t="s">
+    <row r="245" spans="1:9">
+      <c r="A245" t="s">
         <v>131</v>
       </c>
-      <c r="B237" s="5">
+      <c r="B245" s="5">
         <v>2.5449999999999999</v>
       </c>
-      <c r="C237" s="5">
+      <c r="C245" s="5">
         <v>2.6150000000000002</v>
       </c>
-      <c r="D237" s="5">
-        <f t="shared" ref="D237" si="162">(C237-B237)/2</f>
+      <c r="D245" s="5">
+        <f t="shared" ref="D245" si="174">(C245-B245)/2</f>
         <v>3.5000000000000142E-2</v>
       </c>
-      <c r="E237" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F237" s="5">
-        <f t="shared" ref="F237" si="163">C237+E237</f>
+      <c r="E245" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F245" s="5">
+        <f t="shared" ref="F245" si="175">C245+E245</f>
         <v>2.6180000000000003</v>
       </c>
-      <c r="G237" s="5">
-        <f t="shared" ref="G237" si="164">B237-E237</f>
+      <c r="G245" s="5">
+        <f t="shared" ref="G245" si="176">B245-E245</f>
         <v>2.5419999999999998</v>
       </c>
-      <c r="H237" t="s">
+      <c r="H245" t="s">
         <v>234</v>
       </c>
-      <c r="I237" s="6" t="s">
+      <c r="I245" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
-      <c r="A238" t="s">
+    <row r="246" spans="1:9">
+      <c r="A246" t="s">
         <v>132</v>
       </c>
-      <c r="B238" s="5">
+      <c r="B246" s="5">
         <v>2.8849999999999998</v>
       </c>
-      <c r="C238" s="5">
+      <c r="C246" s="5">
         <v>2.9950000000000001</v>
       </c>
-      <c r="D238" s="5">
-        <f t="shared" ref="D238" si="165">(C238-B238)/2</f>
+      <c r="D246" s="5">
+        <f t="shared" ref="D246" si="177">(C246-B246)/2</f>
         <v>5.500000000000016E-2</v>
       </c>
-      <c r="E238" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F238" s="5">
-        <f t="shared" ref="F238" si="166">C238+E238</f>
+      <c r="E246" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F246" s="5">
+        <f t="shared" ref="F246" si="178">C246+E246</f>
         <v>2.9980000000000002</v>
       </c>
-      <c r="G238" s="5">
-        <f t="shared" ref="G238" si="167">B238-E238</f>
+      <c r="G246" s="5">
+        <f t="shared" ref="G246" si="179">B246-E246</f>
         <v>2.8819999999999997</v>
       </c>
-      <c r="H238" t="s">
+      <c r="H246" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
-      <c r="A239" t="s">
+    <row r="247" spans="1:9">
+      <c r="A247" t="s">
         <v>235</v>
       </c>
-      <c r="B239" s="5">
+      <c r="B247" s="5">
         <v>3.7850000000000001</v>
       </c>
-      <c r="C239" s="5">
+      <c r="C247" s="5">
         <v>3.895</v>
       </c>
-      <c r="D239" s="5">
-        <f t="shared" ref="D239" si="168">(C239-B239)/2</f>
+      <c r="D247" s="5">
+        <f t="shared" ref="D247" si="180">(C247-B247)/2</f>
         <v>5.4999999999999938E-2</v>
       </c>
-      <c r="E239" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F239" s="5">
-        <f t="shared" ref="F239" si="169">C239+E239</f>
+      <c r="E247" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F247" s="5">
+        <f t="shared" ref="F247" si="181">C247+E247</f>
         <v>3.8980000000000001</v>
       </c>
-      <c r="G239" s="5">
-        <f t="shared" ref="G239" si="170">B239-E239</f>
+      <c r="G247" s="5">
+        <f t="shared" ref="G247" si="182">B247-E247</f>
         <v>3.782</v>
       </c>
-      <c r="H239" t="s">
+      <c r="H247" t="s">
         <v>265</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update blue tube data in body_tube_data.xlsx
</commit_message>
<xml_diff>
--- a/data/body_tube_data.xlsx
+++ b/data/body_tube_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2360" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3480" yWindow="2360" windowWidth="28720" windowHeight="28120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="314">
   <si>
     <t>ID inches</t>
   </si>
@@ -1012,7 +1012,13 @@
     <t>7.5 in</t>
   </si>
   <si>
-    <t>Sizes all from Always Ready Rocketry site 2017</t>
+    <t>available in 48 and 72 inch lengths</t>
+  </si>
+  <si>
+    <t>ref alwaysreadyrocketry.com 2017</t>
+  </si>
+  <si>
+    <t>48 in length</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1128,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1214,6 +1220,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1437,7 +1447,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="293">
     <cellStyle name="20% - Accent1" xfId="90" builtinId="30"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1582,6 +1592,8 @@
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1726,6 +1738,8 @@
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2057,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4072,6 +4086,9 @@
       <c r="A98" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="H98" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="1"/>
@@ -4131,7 +4148,7 @@
         <v>1.147</v>
       </c>
       <c r="H101" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4159,6 +4176,9 @@
         <f t="shared" si="26"/>
         <v>1.5170000000000001</v>
       </c>
+      <c r="H102" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
@@ -4185,6 +4205,9 @@
         <f t="shared" si="26"/>
         <v>2.1469999999999998</v>
       </c>
+      <c r="H103" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
@@ -4211,6 +4234,9 @@
         <f t="shared" si="26"/>
         <v>2.5569999999999999</v>
       </c>
+      <c r="H104" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
@@ -4237,6 +4263,9 @@
         <f t="shared" si="26"/>
         <v>2.9969999999999999</v>
       </c>
+      <c r="H105" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
@@ -4263,6 +4292,9 @@
         <f t="shared" si="26"/>
         <v>3.8969999999999998</v>
       </c>
+      <c r="H106" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
@@ -4289,6 +4321,9 @@
         <f t="shared" si="26"/>
         <v>5.4969999999999999</v>
       </c>
+      <c r="H107" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
@@ -4315,6 +4350,9 @@
         <f t="shared" si="26"/>
         <v>5.9969999999999999</v>
       </c>
+      <c r="H108" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
@@ -4340,6 +4378,9 @@
       <c r="G109" s="5">
         <f t="shared" si="26"/>
         <v>7.4969999999999999</v>
+      </c>
+      <c r="H109" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="111" spans="1:9">

</xml_diff>